<commit_message>
Add Excel sheets for data analysis
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise data/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise data/2020_cars_combined.xlsx
@@ -429,42 +429,52 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Default green</t>
+          <t>Toyota Yaris</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Mazda MX-30</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Honda JAZZ</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Land Rover Defender</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>SEAT Leon</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>KIA Sorento</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Default Red</t>
+          <t>Honda e</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Blue</t>
+          <t>Hyundai i10</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>ISUZU D-Max Crew Cab</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Audi A3</t>
         </is>
       </c>
     </row>

</xml_diff>